<commit_message>
Rename 'terminations' to 'targets'
</commit_message>
<xml_diff>
--- a/PSM-hackathon-leaf-flows_annotated.xlsx
+++ b/PSM-hackathon-leaf-flows_annotated.xlsx
@@ -5,12 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="flow" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="quantity" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="terminations" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="targets" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="mass_hints" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames>
@@ -3604,26 +3604,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="true">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:L811"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A200" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="24.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="4" style="0" width="8.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="13.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="10" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26058,7 +26055,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -26068,13 +26065,12 @@
       <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="51.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="38.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26117,25 +26113,23 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:F54"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D24" activeCellId="0" sqref="D24"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E29" activeCellId="0" sqref="E29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.06"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="37.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="40.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="38.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="37.76"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -27014,20 +27008,17 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:I1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.67"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">

</xml_diff>